<commit_message>
Added bar code and corrected reference designators for D4
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP02HYPM_00004.xlsx
+++ b/deployment/Omaha_Cal_Info_GP02HYPM_00004.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="21400" windowHeight="11860"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="21405" windowHeight="11865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="122">
   <si>
     <t>Ref Des</t>
   </si>
@@ -345,6 +350,54 @@
   </si>
   <si>
     <t>3.250000e-06</t>
+  </si>
+  <si>
+    <t>OL000580</t>
+  </si>
+  <si>
+    <t>N00608</t>
+  </si>
+  <si>
+    <t>N00609</t>
+  </si>
+  <si>
+    <t>N00610</t>
+  </si>
+  <si>
+    <t>Serial number doesn’t look accurate</t>
+  </si>
+  <si>
+    <t>OL000581</t>
+  </si>
+  <si>
+    <t>A00631</t>
+  </si>
+  <si>
+    <t>N00604</t>
+  </si>
+  <si>
+    <t>N00605</t>
+  </si>
+  <si>
+    <t>N00606</t>
+  </si>
+  <si>
+    <t>N00607</t>
+  </si>
+  <si>
+    <t>A00267</t>
+  </si>
+  <si>
+    <t>A01767</t>
+  </si>
+  <si>
+    <t>A01766</t>
+  </si>
+  <si>
+    <t>A01394</t>
+  </si>
+  <si>
+    <t>OL000022</t>
   </si>
 </sst>
 </file>
@@ -352,13 +405,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -548,12 +601,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -696,14 +743,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -881,7 +928,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -895,13 +942,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -919,7 +966,7 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -958,7 +1005,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -967,7 +1014,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -976,7 +1023,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1013,7 +1059,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1043,7 +1088,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1318,7 +1363,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1623,30 +1668,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="12.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="28">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="25.5">
       <c r="A1" s="15" t="s">
         <v>43</v>
       </c>
@@ -1684,8 +1729,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="28" customFormat="1">
-      <c r="A2" s="24"/>
+    <row r="2" spans="1:14" s="28" customFormat="1" ht="15">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
       <c r="B2" s="25" t="s">
         <v>40</v>
       </c>
@@ -1725,15 +1772,15 @@
       <c r="F3" s="13"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1">
+    <row r="4" spans="1:14" customFormat="1" ht="15">
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" customFormat="1"/>
-    <row r="6" spans="1:14" customFormat="1"/>
-    <row r="7" spans="1:14" customFormat="1"/>
-    <row r="8" spans="1:14" customFormat="1"/>
-    <row r="9" spans="1:14" customFormat="1"/>
+    <row r="5" spans="1:14" customFormat="1" ht="15"/>
+    <row r="6" spans="1:14" customFormat="1" ht="15"/>
+    <row r="7" spans="1:14" customFormat="1" ht="15"/>
+    <row r="8" spans="1:14" customFormat="1" ht="15"/>
+    <row r="9" spans="1:14" customFormat="1" ht="15"/>
     <row r="10" spans="1:14" s="8" customFormat="1">
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
@@ -1784,29 +1831,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38:F39"/>
+      <selection pane="bottomRight" activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5" style="4" customWidth="1"/>
-    <col min="9" max="13" width="10.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="31" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" style="4" customWidth="1"/>
+    <col min="9" max="13" width="10.7109375" style="4" customWidth="1"/>
     <col min="14" max="14" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="4"/>
+    <col min="15" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="28">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="38.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1845,382 +1892,445 @@
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
     </row>
-    <row r="3" spans="1:9" s="23" customFormat="1">
+    <row r="3" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="31">
         <v>4</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="53">
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="51">
         <v>3283</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="56">
+      <c r="H3" s="54">
         <v>45</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="23" customFormat="1">
-      <c r="A4" s="50" t="s">
+    <row r="4" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="49">
-        <v>4</v>
-      </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="54">
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="47">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="52">
         <v>3283</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="56">
+      <c r="H4" s="54">
         <v>1.716E-6</v>
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" s="23" customFormat="1">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="49">
-        <v>4</v>
-      </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="54">
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="47">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="52">
         <v>3283</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="55">
+      <c r="H5" s="53">
         <v>45</v>
       </c>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" s="23" customFormat="1">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A6" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="49">
-        <v>4</v>
-      </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="54">
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="47">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="52">
         <v>3283</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="55">
+      <c r="H6" s="53">
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" s="23" customFormat="1">
-      <c r="A7" s="50" t="s">
+    <row r="7" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="49">
-        <v>4</v>
-      </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="54">
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="47">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="52">
         <v>3283</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="34">
         <v>140</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="23" customFormat="1">
-      <c r="A8" s="50" t="s">
+    <row r="8" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A8" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="49">
-        <v>4</v>
-      </c>
-      <c r="E8" s="47"/>
-      <c r="F8" s="54">
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="47">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="52">
         <v>3283</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="34">
         <v>700</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="23" customFormat="1">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A9" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="49">
-        <v>4</v>
-      </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="54">
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="47">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="52">
         <v>3283</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="34">
         <v>1.0960000000000001</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="23" customFormat="1">
-      <c r="A10" s="50" t="s">
+    <row r="10" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A10" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="49">
-        <v>4</v>
-      </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="54">
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="47">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="52">
         <v>3283</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="35">
         <v>3.9E-2</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="23" customFormat="1">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
-      <c r="C11" s="41"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="31"/>
       <c r="F11" s="19"/>
-      <c r="G11" s="34"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="18"/>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" spans="1:9" s="23" customFormat="1">
+      <c r="I11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="41" t="s">
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="31">
         <v>4</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="53">
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="51">
         <v>1480</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="59">
+      <c r="H12" s="57">
         <v>50.079599999999999</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="23" customFormat="1">
-      <c r="A13" s="50" t="s">
+    <row r="13" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A13" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="49">
-        <v>4</v>
-      </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="54">
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="47">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="52">
         <v>1480</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="59">
+      <c r="H13" s="57">
         <v>-144.80571666666665</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="23" customFormat="1">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
-      <c r="C14" s="41"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="31"/>
       <c r="F14" s="19"/>
-      <c r="G14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" s="23" customFormat="1">
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="41" t="s">
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D15" s="31">
         <v>4</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="51" t="s">
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="59">
+      <c r="H15" s="57">
         <v>50.079599999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="23" customFormat="1">
-      <c r="A16" s="50" t="s">
+    <row r="16" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A16" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="49">
-        <v>4</v>
-      </c>
-      <c r="E16" s="47"/>
-      <c r="F16" s="52" t="s">
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="47">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="59">
+      <c r="H16" s="57">
         <v>-144.80571666666665</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="23" customFormat="1">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
-      <c r="C17" s="41"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="31"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" s="23" customFormat="1">
+      <c r="G17" s="32"/>
+    </row>
+    <row r="18" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A18" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="41" t="s">
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="31">
         <v>4</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="53">
+      <c r="E18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="51">
         <v>1108</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="59">
+      <c r="H18" s="57">
         <v>50.079599999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="23" customFormat="1">
-      <c r="A19" s="50" t="s">
+      <c r="I18" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A19" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="49">
-        <v>4</v>
-      </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="54">
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="47">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="52">
         <v>1108</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="59">
+      <c r="H19" s="57">
         <v>-144.80571666666665</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="23" customFormat="1">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
-      <c r="C20" s="41"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="31"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="33"/>
-    </row>
-    <row r="21" spans="1:9" s="23" customFormat="1">
-      <c r="A21" s="37" t="s">
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A21" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
       <c r="C21" s="31" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="31">
         <v>4</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="57" t="s">
+      <c r="E21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="55" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2228,1105 +2338,1304 @@
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:9" s="23" customFormat="1">
+    <row r="23" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="41" t="s">
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="31">
         <v>4</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="53">
+      <c r="E23" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="51">
         <v>2736</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="56">
+      <c r="H23" s="54">
         <v>46</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="23" customFormat="1">
-      <c r="A24" s="50" t="s">
+    <row r="24" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A24" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="49">
-        <v>4</v>
-      </c>
-      <c r="E24" s="47"/>
-      <c r="F24" s="54">
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="47">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="52">
         <v>2736</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="56">
+      <c r="H24" s="54">
         <v>1.8279999999999999E-6</v>
       </c>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="1:9" s="23" customFormat="1">
-      <c r="A25" s="50" t="s">
+      <c r="I24" s="32"/>
+    </row>
+    <row r="25" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="49">
-        <v>4</v>
-      </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="54">
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="47">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="52">
         <v>2736</v>
       </c>
-      <c r="G25" s="34" t="s">
+      <c r="G25" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H25" s="53">
         <v>45</v>
       </c>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="1:9" s="23" customFormat="1">
-      <c r="A26" s="50" t="s">
+    <row r="26" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A26" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="49">
-        <v>4</v>
-      </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="54">
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="47">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="52">
         <v>2736</v>
       </c>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H26" s="55">
+      <c r="H26" s="53">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:9" s="23" customFormat="1">
-      <c r="A27" s="50" t="s">
+    <row r="27" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A27" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="49">
-        <v>4</v>
-      </c>
-      <c r="E27" s="47"/>
-      <c r="F27" s="54">
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="47">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="52">
         <v>2736</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G27" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="34">
         <v>140</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="23" customFormat="1">
-      <c r="A28" s="50" t="s">
+    <row r="28" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A28" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="49">
-        <v>4</v>
-      </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="54">
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="47">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="52">
         <v>2736</v>
       </c>
-      <c r="G28" s="34" t="s">
+      <c r="G28" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="34">
         <v>700</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="23" customFormat="1">
-      <c r="A29" s="50" t="s">
+    <row r="29" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A29" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="49">
-        <v>4</v>
-      </c>
-      <c r="E29" s="47"/>
-      <c r="F29" s="54">
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="47">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="52">
         <v>2736</v>
       </c>
-      <c r="G29" s="34" t="s">
+      <c r="G29" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="34">
         <v>1.0960000000000001</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="I29" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="23" customFormat="1">
-      <c r="A30" s="50" t="s">
+    <row r="30" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A30" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="49">
-        <v>4</v>
-      </c>
-      <c r="E30" s="47"/>
-      <c r="F30" s="54">
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="47">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="52">
         <v>2736</v>
       </c>
-      <c r="G30" s="34" t="s">
+      <c r="G30" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="36">
+      <c r="H30" s="35">
         <v>3.9E-2</v>
       </c>
-      <c r="I30" s="34" t="s">
+      <c r="I30" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="23" customFormat="1">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="41"/>
+      <c r="C31" s="40"/>
       <c r="D31" s="31"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="34"/>
+      <c r="G31" s="33"/>
       <c r="H31" s="18"/>
-      <c r="I31" s="34"/>
-    </row>
-    <row r="32" spans="1:9" s="23" customFormat="1">
+      <c r="I31" s="33"/>
+    </row>
+    <row r="32" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A32" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="41" t="s">
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D32" s="31">
         <v>4</v>
       </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="53">
+      <c r="E32" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="51">
         <v>1086</v>
       </c>
-      <c r="G32" s="33" t="s">
+      <c r="G32" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="59">
+      <c r="H32" s="57">
         <v>50.079599999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="23" customFormat="1">
-      <c r="A33" s="50" t="s">
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A33" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="49">
-        <v>4</v>
-      </c>
-      <c r="E33" s="47"/>
-      <c r="F33" s="54">
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="47">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="52">
         <v>1086</v>
       </c>
-      <c r="G33" s="33" t="s">
+      <c r="G33" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="59">
+      <c r="H33" s="57">
         <v>-144.80571666666665</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="23" customFormat="1">
+    <row r="34" spans="1:9" s="23" customFormat="1">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="41"/>
+      <c r="C34" s="40"/>
       <c r="D34" s="31"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="33"/>
-    </row>
-    <row r="35" spans="1:12" s="23" customFormat="1">
+      <c r="G34" s="32"/>
+    </row>
+    <row r="35" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A35" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="41" t="s">
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D35" s="31">
         <v>4</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="51" t="s">
+      <c r="E35" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="33" t="s">
+      <c r="G35" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="59">
+      <c r="H35" s="57">
         <v>50.079599999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="23" customFormat="1">
-      <c r="A36" s="50" t="s">
+    <row r="36" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A36" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="49">
-        <v>4</v>
-      </c>
-      <c r="E36" s="47"/>
-      <c r="F36" s="54" t="s">
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="47">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="33" t="s">
+      <c r="G36" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="59">
+      <c r="H36" s="57">
         <v>-144.80571666666665</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="23" customFormat="1">
+    <row r="37" spans="1:9" s="23" customFormat="1">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="41"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="31"/>
       <c r="F37" s="19"/>
-      <c r="G37" s="33"/>
-    </row>
-    <row r="38" spans="1:12" s="23" customFormat="1">
+      <c r="G37" s="32"/>
+    </row>
+    <row r="38" spans="1:9" s="23" customFormat="1" ht="15">
       <c r="A38" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="41" t="s">
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D38" s="31">
         <v>4</v>
       </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="51" t="s">
+      <c r="E38" t="s">
+        <v>116</v>
+      </c>
+      <c r="F38" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="G38" s="33" t="s">
+      <c r="G38" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H38" s="59">
+      <c r="H38" s="57">
         <v>50.079599999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="23" customFormat="1">
-      <c r="A39" s="50" t="s">
+    <row r="39" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A39" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="47"/>
-      <c r="C39" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="49">
-        <v>4</v>
-      </c>
-      <c r="E39" s="47"/>
-      <c r="F39" s="52" t="s">
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="47">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="G39" s="33" t="s">
+      <c r="G39" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="59">
+      <c r="H39" s="57">
         <v>-144.80571666666665</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="23" customFormat="1">
+    <row r="40" spans="1:9" s="23" customFormat="1">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
-      <c r="C40" s="41"/>
+      <c r="C40" s="40"/>
       <c r="D40" s="31"/>
       <c r="F40" s="19"/>
-      <c r="G40" s="33"/>
-    </row>
-    <row r="41" spans="1:12" s="23" customFormat="1">
-      <c r="A41" s="37" t="s">
+      <c r="G40" s="32"/>
+    </row>
+    <row r="41" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A41" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
       <c r="C41" s="31" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="31">
         <v>4</v>
       </c>
-      <c r="E41" s="32"/>
-      <c r="F41" s="57" t="s">
+      <c r="E41" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41" s="55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="23" customFormat="1">
+    <row r="42" spans="1:9" s="23" customFormat="1">
       <c r="C42" s="31"/>
       <c r="D42" s="31"/>
     </row>
-    <row r="43" spans="1:12" s="23" customFormat="1">
-      <c r="A43" s="38" t="s">
+    <row r="43" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A43" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="41" t="s">
+      <c r="B43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D43" s="31">
         <v>4</v>
       </c>
-      <c r="F43" s="42" t="s">
+      <c r="E43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="I43" s="39" t="s">
+      <c r="I43" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="L43" s="21"/>
-    </row>
-    <row r="44" spans="1:12" s="23" customFormat="1">
-      <c r="A44" s="38"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="41"/>
+    </row>
+    <row r="44" spans="1:9" s="23" customFormat="1">
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="31"/>
       <c r="F44" s="21"/>
-      <c r="I44" s="39"/>
-    </row>
-    <row r="45" spans="1:12" s="23" customFormat="1">
-      <c r="A45" s="38" t="s">
+      <c r="I44" s="38"/>
+    </row>
+    <row r="45" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A45" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="41" t="s">
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D45" s="31">
         <v>4</v>
       </c>
-      <c r="F45" s="42" t="s">
+      <c r="E45" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="I45" s="39" t="s">
+      <c r="I45" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="L45" s="21"/>
-    </row>
-    <row r="46" spans="1:12" s="23" customFormat="1">
-      <c r="A46" s="38"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="41"/>
+    </row>
+    <row r="46" spans="1:9" s="23" customFormat="1">
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="31"/>
       <c r="F46" s="21"/>
-      <c r="I46" s="39"/>
-    </row>
-    <row r="47" spans="1:12" s="23" customFormat="1">
-      <c r="A47" s="37" t="s">
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A47" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="41" t="str">
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="40" t="str">
         <f>$C$4</f>
         <v>GP02HYPM-00004</v>
       </c>
       <c r="D47" s="31">
         <v>4</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="57" t="s">
+      <c r="E47" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" s="55" t="s">
         <v>79</v>
       </c>
       <c r="G47" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="59">
+      <c r="H47" s="57">
         <v>50.079599999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="23" customFormat="1">
-      <c r="A48" s="46" t="s">
+    <row r="48" spans="1:9" s="23" customFormat="1" ht="15">
+      <c r="A48" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="47"/>
-      <c r="C48" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" s="49">
-        <v>4</v>
-      </c>
-      <c r="E48" s="47"/>
-      <c r="F48" s="58" t="s">
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="47">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F48" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G48" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="59">
+      <c r="H48" s="57">
         <v>-144.80571666666665</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="23" customFormat="1">
-      <c r="A49" s="46" t="s">
+    <row r="49" spans="1:12" s="23" customFormat="1" ht="15">
+      <c r="A49" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="47"/>
-      <c r="C49" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="49">
-        <v>4</v>
-      </c>
-      <c r="E49" s="47"/>
-      <c r="F49" s="58" t="s">
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="47">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G49" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="56">
+      <c r="H49" s="54">
         <v>1450</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="43" customFormat="1">
-      <c r="A50" s="46" t="s">
+    <row r="50" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A50" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D50" s="49">
-        <v>4</v>
-      </c>
-      <c r="E50" s="47"/>
-      <c r="F50" s="58" t="s">
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="47">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H50" s="60" t="s">
+      <c r="H50" s="58" t="s">
         <v>83</v>
       </c>
       <c r="I50" s="4"/>
-    </row>
-    <row r="51" spans="1:11" s="43" customFormat="1">
-      <c r="A51" s="46" t="s">
+      <c r="L50" s="23"/>
+    </row>
+    <row r="51" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A51" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" s="49">
-        <v>4</v>
-      </c>
-      <c r="E51" s="47"/>
-      <c r="F51" s="58" t="s">
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="47">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H51" s="61" t="s">
+      <c r="H51" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="I51" s="44"/>
-      <c r="K51" s="45"/>
-    </row>
-    <row r="52" spans="1:11" s="43" customFormat="1">
-      <c r="A52" s="46" t="s">
+      <c r="I51" s="43"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="23"/>
+    </row>
+    <row r="52" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A52" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="49">
-        <v>4</v>
-      </c>
-      <c r="E52" s="47"/>
-      <c r="F52" s="58" t="s">
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="47">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>120</v>
+      </c>
+      <c r="F52" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H52" s="61" t="s">
+      <c r="H52" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="I52" s="44"/>
-      <c r="K52" s="45"/>
-    </row>
-    <row r="53" spans="1:11" s="43" customFormat="1">
-      <c r="A53" s="46" t="s">
+      <c r="I52" s="43"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="23"/>
+    </row>
+    <row r="53" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A53" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="47"/>
-      <c r="C53" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="49">
-        <v>4</v>
-      </c>
-      <c r="E53" s="47"/>
-      <c r="F53" s="58" t="s">
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="47">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H53" s="61" t="s">
+      <c r="H53" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="I53" s="44"/>
-      <c r="K53" s="45"/>
-    </row>
-    <row r="54" spans="1:11" s="43" customFormat="1">
-      <c r="A54" s="46" t="s">
+      <c r="I53" s="43"/>
+      <c r="K53" s="44"/>
+      <c r="L53" s="23"/>
+    </row>
+    <row r="54" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A54" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="47"/>
-      <c r="C54" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D54" s="49">
-        <v>4</v>
-      </c>
-      <c r="E54" s="47"/>
-      <c r="F54" s="58" t="s">
+      <c r="B54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="47">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H54" s="61" t="s">
+      <c r="H54" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="I54" s="44"/>
-      <c r="K54" s="45"/>
-    </row>
-    <row r="55" spans="1:11" s="43" customFormat="1">
-      <c r="A55" s="46" t="s">
+      <c r="I54" s="43"/>
+      <c r="K54" s="44"/>
+      <c r="L54" s="23"/>
+    </row>
+    <row r="55" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A55" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="47"/>
-      <c r="C55" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D55" s="49">
-        <v>4</v>
-      </c>
-      <c r="E55" s="47"/>
-      <c r="F55" s="58" t="s">
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" s="47">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H55" s="62" t="s">
+      <c r="H55" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="I55" s="44"/>
-      <c r="K55" s="45"/>
-    </row>
-    <row r="56" spans="1:11" s="43" customFormat="1">
-      <c r="A56" s="46" t="s">
+      <c r="I55" s="43"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="23"/>
+    </row>
+    <row r="56" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A56" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="47"/>
-      <c r="C56" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D56" s="49">
-        <v>4</v>
-      </c>
-      <c r="E56" s="47"/>
-      <c r="F56" s="58" t="s">
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="47">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>120</v>
+      </c>
+      <c r="F56" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H56" s="62" t="s">
+      <c r="H56" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="I56" s="44"/>
-      <c r="K56" s="45"/>
-    </row>
-    <row r="57" spans="1:11" s="43" customFormat="1">
-      <c r="A57" s="46" t="s">
+      <c r="I56" s="43"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="23"/>
+    </row>
+    <row r="57" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A57" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="49">
-        <v>4</v>
-      </c>
-      <c r="E57" s="47"/>
-      <c r="F57" s="58" t="s">
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="47">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H57" s="62" t="s">
+      <c r="H57" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="I57" s="44"/>
-      <c r="K57" s="45"/>
-    </row>
-    <row r="58" spans="1:11" s="43" customFormat="1">
-      <c r="A58" s="46" t="s">
+      <c r="I57" s="43"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="23"/>
+    </row>
+    <row r="58" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A58" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="49">
-        <v>4</v>
-      </c>
-      <c r="E58" s="47"/>
-      <c r="F58" s="58" t="s">
+      <c r="B58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="47">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H58" s="62" t="s">
+      <c r="H58" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="I58" s="44"/>
-      <c r="K58" s="45"/>
-    </row>
-    <row r="59" spans="1:11" s="43" customFormat="1">
-      <c r="A59" s="46" t="s">
+      <c r="I58" s="43"/>
+      <c r="K58" s="44"/>
+      <c r="L58" s="23"/>
+    </row>
+    <row r="59" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A59" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="47"/>
-      <c r="C59" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D59" s="49">
-        <v>4</v>
-      </c>
-      <c r="E59" s="47"/>
-      <c r="F59" s="58" t="s">
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="47">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H59" s="62" t="s">
+      <c r="H59" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="I59" s="44"/>
-      <c r="K59" s="45"/>
-    </row>
-    <row r="60" spans="1:11" s="43" customFormat="1">
-      <c r="A60" s="46" t="s">
+      <c r="I59" s="43"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="23"/>
+    </row>
+    <row r="60" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A60" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="47"/>
-      <c r="C60" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D60" s="49">
-        <v>4</v>
-      </c>
-      <c r="E60" s="47"/>
-      <c r="F60" s="58" t="s">
+      <c r="B60" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" s="47">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H60" s="62" t="s">
+      <c r="H60" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="I60" s="44"/>
-      <c r="K60" s="45"/>
-    </row>
-    <row r="61" spans="1:11" s="43" customFormat="1">
-      <c r="A61" s="46" t="s">
+      <c r="I60" s="43"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="23"/>
+    </row>
+    <row r="61" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A61" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B61" s="47"/>
-      <c r="C61" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" s="49">
-        <v>4</v>
-      </c>
-      <c r="E61" s="47"/>
-      <c r="F61" s="58" t="s">
+      <c r="B61" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="47">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H61" s="62" t="s">
+      <c r="H61" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="I61" s="44"/>
-      <c r="K61" s="45"/>
-    </row>
-    <row r="62" spans="1:11" s="43" customFormat="1">
-      <c r="A62" s="46" t="s">
+      <c r="I61" s="43"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="23"/>
+    </row>
+    <row r="62" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A62" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="47"/>
-      <c r="C62" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="49">
-        <v>4</v>
-      </c>
-      <c r="E62" s="47"/>
-      <c r="F62" s="58" t="s">
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" s="47">
+        <v>4</v>
+      </c>
+      <c r="E62" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H62" s="62" t="s">
+      <c r="H62" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="I62" s="44"/>
-      <c r="K62" s="45"/>
-    </row>
-    <row r="63" spans="1:11" s="43" customFormat="1">
-      <c r="A63" s="46" t="s">
+      <c r="I62" s="43"/>
+      <c r="K62" s="44"/>
+      <c r="L62" s="23"/>
+    </row>
+    <row r="63" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A63" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B63" s="47"/>
-      <c r="C63" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D63" s="49">
-        <v>4</v>
-      </c>
-      <c r="E63" s="47"/>
-      <c r="F63" s="58" t="s">
+      <c r="B63" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="47">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H63" s="62" t="s">
+      <c r="H63" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I63" s="44"/>
-      <c r="K63" s="45"/>
-    </row>
-    <row r="64" spans="1:11" s="43" customFormat="1">
-      <c r="A64" s="46" t="s">
+      <c r="I63" s="43"/>
+      <c r="K63" s="44"/>
+      <c r="L63" s="23"/>
+    </row>
+    <row r="64" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A64" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B64" s="47"/>
-      <c r="C64" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D64" s="49">
-        <v>4</v>
-      </c>
-      <c r="E64" s="47"/>
-      <c r="F64" s="58" t="s">
+      <c r="B64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="47">
+        <v>4</v>
+      </c>
+      <c r="E64" t="s">
+        <v>120</v>
+      </c>
+      <c r="F64" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H64" s="62" t="s">
+      <c r="H64" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="I64" s="44"/>
-      <c r="K64" s="45"/>
-    </row>
-    <row r="65" spans="1:11" s="43" customFormat="1">
-      <c r="A65" s="46" t="s">
+      <c r="I64" s="43"/>
+      <c r="K64" s="44"/>
+      <c r="L64" s="23"/>
+    </row>
+    <row r="65" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A65" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B65" s="47"/>
-      <c r="C65" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D65" s="49">
-        <v>4</v>
-      </c>
-      <c r="E65" s="47"/>
-      <c r="F65" s="58" t="s">
+      <c r="B65" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="47">
+        <v>4</v>
+      </c>
+      <c r="E65" t="s">
+        <v>120</v>
+      </c>
+      <c r="F65" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H65" s="62" t="s">
+      <c r="H65" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="I65" s="44"/>
-      <c r="K65" s="45"/>
-    </row>
-    <row r="66" spans="1:11" s="43" customFormat="1">
-      <c r="A66" s="46" t="s">
+      <c r="I65" s="43"/>
+      <c r="K65" s="44"/>
+      <c r="L65" s="23"/>
+    </row>
+    <row r="66" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A66" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B66" s="47"/>
-      <c r="C66" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D66" s="49">
-        <v>4</v>
-      </c>
-      <c r="E66" s="47"/>
-      <c r="F66" s="58" t="s">
+      <c r="B66" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="47">
+        <v>4</v>
+      </c>
+      <c r="E66" t="s">
+        <v>120</v>
+      </c>
+      <c r="F66" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H66" s="62" t="s">
+      <c r="H66" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="I66" s="44"/>
-      <c r="K66" s="45"/>
-    </row>
-    <row r="67" spans="1:11" s="43" customFormat="1">
-      <c r="A67" s="46" t="s">
+      <c r="I66" s="43"/>
+      <c r="K66" s="44"/>
+      <c r="L66" s="23"/>
+    </row>
+    <row r="67" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A67" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="47"/>
-      <c r="C67" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" s="49">
-        <v>4</v>
-      </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="58" t="s">
+      <c r="B67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="47">
+        <v>4</v>
+      </c>
+      <c r="E67" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H67" s="62" t="s">
+      <c r="H67" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="I67" s="44"/>
-      <c r="K67" s="45"/>
-    </row>
-    <row r="68" spans="1:11" s="43" customFormat="1">
-      <c r="A68" s="46" t="s">
+      <c r="I67" s="43"/>
+      <c r="K67" s="44"/>
+      <c r="L67" s="23"/>
+    </row>
+    <row r="68" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A68" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B68" s="47"/>
-      <c r="C68" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D68" s="49">
-        <v>4</v>
-      </c>
-      <c r="E68" s="47"/>
-      <c r="F68" s="58" t="s">
+      <c r="B68" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="47">
+        <v>4</v>
+      </c>
+      <c r="E68" t="s">
+        <v>120</v>
+      </c>
+      <c r="F68" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H68" s="62" t="s">
+      <c r="H68" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="I68" s="44"/>
-      <c r="K68" s="45"/>
-    </row>
-    <row r="69" spans="1:11" s="43" customFormat="1">
-      <c r="A69" s="46" t="s">
+      <c r="I68" s="43"/>
+      <c r="K68" s="44"/>
+      <c r="L68" s="23"/>
+    </row>
+    <row r="69" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A69" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B69" s="47"/>
-      <c r="C69" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D69" s="49">
-        <v>4</v>
-      </c>
-      <c r="E69" s="47"/>
-      <c r="F69" s="58" t="s">
+      <c r="B69" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D69" s="47">
+        <v>4</v>
+      </c>
+      <c r="E69" t="s">
+        <v>120</v>
+      </c>
+      <c r="F69" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H69" s="62" t="s">
+      <c r="H69" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="I69" s="44"/>
-      <c r="K69" s="45"/>
-    </row>
-    <row r="70" spans="1:11" s="43" customFormat="1">
-      <c r="A70" s="46" t="s">
+      <c r="I69" s="43"/>
+      <c r="K69" s="44"/>
+      <c r="L69" s="23"/>
+    </row>
+    <row r="70" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A70" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B70" s="47"/>
-      <c r="C70" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D70" s="49">
-        <v>4</v>
-      </c>
-      <c r="E70" s="47"/>
-      <c r="F70" s="58" t="s">
+      <c r="B70" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="47">
+        <v>4</v>
+      </c>
+      <c r="E70" t="s">
+        <v>120</v>
+      </c>
+      <c r="F70" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H70" s="62" t="s">
+      <c r="H70" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="I70" s="44"/>
-      <c r="K70" s="45"/>
-    </row>
-    <row r="71" spans="1:11" s="43" customFormat="1">
-      <c r="A71" s="46" t="s">
+      <c r="I70" s="43"/>
+      <c r="K70" s="44"/>
+      <c r="L70" s="23"/>
+    </row>
+    <row r="71" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A71" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B71" s="47"/>
-      <c r="C71" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D71" s="49">
-        <v>4</v>
-      </c>
-      <c r="E71" s="47"/>
-      <c r="F71" s="58" t="s">
+      <c r="B71" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D71" s="47">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>120</v>
+      </c>
+      <c r="F71" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H71" s="62" t="s">
+      <c r="H71" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="I71" s="44"/>
-      <c r="K71" s="45"/>
-    </row>
-    <row r="72" spans="1:11" s="43" customFormat="1">
-      <c r="A72" s="46" t="s">
+      <c r="I71" s="43"/>
+      <c r="K71" s="44"/>
+      <c r="L71" s="23"/>
+    </row>
+    <row r="72" spans="1:12" s="42" customFormat="1" ht="15">
+      <c r="A72" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B72" s="47"/>
-      <c r="C72" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D72" s="49">
-        <v>4</v>
-      </c>
-      <c r="E72" s="47"/>
-      <c r="F72" s="58" t="s">
+      <c r="B72" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="47">
+        <v>4</v>
+      </c>
+      <c r="E72" t="s">
+        <v>120</v>
+      </c>
+      <c r="F72" s="56" t="s">
         <v>79</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H72" s="62" t="s">
+      <c r="H72" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="I72" s="44"/>
-      <c r="K72" s="45"/>
-    </row>
-    <row r="73" spans="1:11" s="23" customFormat="1">
+      <c r="I72" s="43"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="23"/>
+    </row>
+    <row r="73" spans="1:12" s="23" customFormat="1">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
-      <c r="C73" s="41"/>
+      <c r="C73" s="40"/>
       <c r="D73" s="31"/>
       <c r="F73" s="19"/>
       <c r="G73" s="22"/>
     </row>
-    <row r="74" spans="1:11" s="23" customFormat="1">
-      <c r="A74" s="40" t="s">
+    <row r="74" spans="1:12" s="23" customFormat="1" ht="15">
+      <c r="A74" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B74" s="32"/>
+      <c r="B74" t="s">
+        <v>106</v>
+      </c>
       <c r="C74" s="31" t="s">
         <v>46</v>
       </c>
       <c r="D74" s="31">
         <v>4</v>
       </c>
-      <c r="E74" s="32"/>
-      <c r="F74" s="42">
+      <c r="E74" t="s">
+        <v>121</v>
+      </c>
+      <c r="F74" s="41">
         <v>12369</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="23" customFormat="1">
-      <c r="A75" s="37"/>
-      <c r="B75" s="37"/>
+    <row r="75" spans="1:12" s="23" customFormat="1">
+      <c r="A75" s="36"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="31"/>
       <c r="D75" s="31"/>
     </row>
-    <row r="76" spans="1:11" s="23" customFormat="1">
+    <row r="76" spans="1:12" s="23" customFormat="1">
       <c r="C76" s="31"/>
       <c r="D76" s="31"/>
     </row>
-    <row r="77" spans="1:11" s="23" customFormat="1">
+    <row r="77" spans="1:12" s="23" customFormat="1">
       <c r="C77" s="31"/>
       <c r="D77" s="31"/>
     </row>
-    <row r="78" spans="1:11" s="23" customFormat="1">
+    <row r="78" spans="1:12" s="23" customFormat="1">
       <c r="C78" s="31"/>
       <c r="D78" s="31"/>
     </row>
-    <row r="79" spans="1:11" s="23" customFormat="1">
+    <row r="79" spans="1:12" s="23" customFormat="1">
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
     </row>
-    <row r="80" spans="1:11" s="23" customFormat="1">
+    <row r="80" spans="1:12" s="23" customFormat="1">
       <c r="C80" s="31"/>
       <c r="D80" s="31"/>
     </row>
@@ -3388,7 +3697,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>